<commit_message>
Updated API spec sheet
</commit_message>
<xml_diff>
--- a/UserMgmtSvc API specification.xlsx
+++ b/UserMgmtSvc API specification.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\WebDev\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\WebDev\WebDevNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="API Specification" sheetId="1" r:id="rId1"/>
+    <sheet name="Details" sheetId="2" r:id="rId2"/>
+    <sheet name="UserMgmt ReactApp" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t>User Mangement Service</t>
   </si>
@@ -392,13 +393,64 @@
   </si>
   <si>
     <t>/deleteUser?userId=123</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Repository Details</t>
+  </si>
+  <si>
+    <t>https://github.com/Krunaljumde24/user-mgmt-react-app.git</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Commit Message</t>
+  </si>
+  <si>
+    <t>v1.00</t>
+  </si>
+  <si>
+    <t>Created UI for user management application</t>
+  </si>
+  <si>
+    <t>Initial commit, project setup of react app, created to components - 1.AddUser 2.Users and used react-hook-form</t>
+  </si>
+  <si>
+    <t>user-mgmt-react-appPublic</t>
+  </si>
+  <si>
+    <t>v1.01</t>
+  </si>
+  <si>
+    <t>Made API calls, GET-/users-to fetch the user data and rendered on tables, POST-/addUser-to add new user from UI to database</t>
+  </si>
+  <si>
+    <t>v1.02</t>
+  </si>
+  <si>
+    <t>Tried to call an API using XMLHttpRequest, but couldn't make POST API call</t>
+  </si>
+  <si>
+    <t>Just trying different HTTP client tools to execute APIs. I'll again try to figure out the approriate usage</t>
+  </si>
+  <si>
+    <t>Used AXIOS http client tool to execute APIs from react app.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,13 +505,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -490,7 +556,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -504,13 +570,34 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -794,7 +881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -808,39 +895,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -940,7 +1027,7 @@
   <dimension ref="B4:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D14"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,4 +1209,108 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5703125" customWidth="1"/>
+    <col min="6" max="6" width="41" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="18"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>